<commit_message>
Winkel finden und auf Töggel zunächst 5cm, später max 1cm drauf zu fahren Neue Fahrwerk::fahrVorwaerts(int p_iSpeed, int p_iDistanceInCm)
</commit_message>
<xml_diff>
--- a/Doku/Schnittestelle_SuchServo_Fahrwerk.xlsx
+++ b/Doku/Schnittestelle_SuchServo_Fahrwerk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Umrechnung Winkel in Motorlaufzeit</t>
   </si>
@@ -38,22 +38,22 @@
     <t>Nächster Töggel gemäss Servo in Grad</t>
   </si>
   <si>
-    <t>Wenn positiv lenkeLinks  um Betrag von Delta</t>
-  </si>
-  <si>
-    <t>Wenn negativ lenkeRechts um Betrag von Delta</t>
-  </si>
-  <si>
     <t>Delay</t>
   </si>
   <si>
     <t>Index in Array</t>
   </si>
   <si>
-    <t>Wenn Array Index zwischen 5 und 9 lenke Rechts um Winkel -45</t>
+    <t>Wenn Winkel &gt; 45 lenke Rechts</t>
   </si>
   <si>
-    <t>Wenn Array Index zwischen 0 und 4 lenke Links um 45 - Winkel</t>
+    <t>Sonst lenke Links</t>
+  </si>
+  <si>
+    <t>Geradeausfahren: Umrechnung cm in delay</t>
+  </si>
+  <si>
+    <t>cm</t>
   </si>
 </sst>
 </file>
@@ -69,12 +69,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -253,7 +260,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15000</c:v>
+                  <c:v>8850</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -452,7 +459,403 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Delay</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$29:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$30:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-053A-4446-8A1F-B64B97E76732}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="465970640"/>
+        <c:axId val="465970968"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="465970640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="465970968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="465970968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="465970640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1008,6 +1411,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1041,6 +1960,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12CD93BA-3A6E-4DDF-9656-417C22B087F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1346,10 +2301,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:R14"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,14 +2312,14 @@
     <col min="7" max="7" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H5">
         <v>9</v>
@@ -1508,29 +2463,48 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>15000</v>
+        <v>8850</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I14" t="s">
-        <v>8</v>
-      </c>
-      <c r="O14" t="s">
-        <v>9</v>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>4100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MOD:  - Neigungssensor TestIBN  - Messdaten Fahrwer auf Distanz in Excel
</commit_message>
<xml_diff>
--- a/Doku/Schnittestelle_SuchServo_Fahrwerk.xlsx
+++ b/Doku/Schnittestelle_SuchServo_Fahrwerk.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10590"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10590" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Fahrversuche" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Umrechnung Winkel in Motorlaufzeit</t>
   </si>
@@ -54,6 +55,45 @@
   </si>
   <si>
     <t>cm</t>
+  </si>
+  <si>
+    <t>delay</t>
+  </si>
+  <si>
+    <t>Richtung</t>
+  </si>
+  <si>
+    <t>geradeaus hoch</t>
+  </si>
+  <si>
+    <t>geradeaus runter</t>
+  </si>
+  <si>
+    <t>links nach rechts</t>
+  </si>
+  <si>
+    <t>rechts nach links</t>
+  </si>
+  <si>
+    <t>diagonal links oben rechts unten</t>
+  </si>
+  <si>
+    <t>diagonal rechts oben links unten</t>
+  </si>
+  <si>
+    <t>Distanz gefahren [cm]</t>
+  </si>
+  <si>
+    <t>diagonal links unten rechts oben</t>
+  </si>
+  <si>
+    <t>diagonal rechts unten links oben</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>SPEED_GANZLANGSAM</t>
   </si>
 </sst>
 </file>
@@ -2303,7 +2343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -2511,4 +2551,135 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>7.5</v>
+      </c>
+      <c r="E2">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>11.5</v>
+      </c>
+      <c r="E5">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>9.5</v>
+      </c>
+      <c r="E7">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>10.5</v>
+      </c>
+      <c r="E9">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fahrwerk kalibiert auf Zielumgebung
</commit_message>
<xml_diff>
--- a/Doku/Schnittestelle_SuchServo_Fahrwerk.xlsx
+++ b/Doku/Schnittestelle_SuchServo_Fahrwerk.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10590" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10590"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -656,7 +656,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4100</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2343,7 +2343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -2544,7 +2544,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <v>4100</v>
+        <v>2100</v>
       </c>
     </row>
   </sheetData>
@@ -2557,7 +2557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
MOD:  - Stand ohne Ultraschall / Servo aus ZBW fixiert
</commit_message>
<xml_diff>
--- a/Doku/Schnittestelle_SuchServo_Fahrwerk.xlsx
+++ b/Doku/Schnittestelle_SuchServo_Fahrwerk.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10590"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10590" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Umrechnung Winkel in Motorlaufzeit</t>
   </si>
@@ -94,6 +94,39 @@
   </si>
   <si>
     <t>SPEED_GANZLANGSAM</t>
+  </si>
+  <si>
+    <t>Mit Zielsystem</t>
+  </si>
+  <si>
+    <t>(delay Faktor 210</t>
+  </si>
+  <si>
+    <t>aufwärts</t>
+  </si>
+  <si>
+    <t>Angabe in cm</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>tatsächlich gefahren:</t>
+  </si>
+  <si>
+    <t>Abweichung max</t>
+  </si>
+  <si>
+    <t>Abweichung min</t>
+  </si>
+  <si>
+    <t>Abweichung mittel</t>
+  </si>
+  <si>
+    <t>Faktor</t>
   </si>
 </sst>
 </file>
@@ -300,7 +333,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8850</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2343,8 +2376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2509,7 +2542,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>8850</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2555,20 +2588,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2582,7 +2622,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4100</v>
       </c>
@@ -2599,7 +2639,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>13</v>
       </c>
@@ -2610,7 +2650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>14</v>
       </c>
@@ -2624,7 +2664,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>15</v>
       </c>
@@ -2635,7 +2675,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>16</v>
       </c>
@@ -2646,7 +2686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>17</v>
       </c>
@@ -2657,7 +2697,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>19</v>
       </c>
@@ -2668,7 +2708,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>20</v>
       </c>
@@ -2677,6 +2717,76 @@
       </c>
       <c r="E9">
         <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>40</v>
+      </c>
+      <c r="E13">
+        <v>26</v>
+      </c>
+      <c r="F13">
+        <v>30</v>
+      </c>
+      <c r="G13">
+        <f>D13-E13</f>
+        <v>14</v>
+      </c>
+      <c r="H13">
+        <f>D13-F13</f>
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <f>(G13+H13)/2</f>
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <f>I13/D13</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <f>E13+E13*J13</f>
+        <v>33.799999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>